<commit_message>
fix musicians and get_studio_lead_vocals service
</commit_message>
<xml_diff>
--- a/scripts/data_sources/musicians.xlsx
+++ b/scripts/data_sources/musicians.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Videos\santanarchive\ms-santanarchive-python\scripts\data_sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$G$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$G$47</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="125">
   <si>
     <t>Nombre</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Guitar, Vocals, Percussion</t>
   </si>
   <si>
-    <t>Presente</t>
-  </si>
-  <si>
     <t>Gregg</t>
   </si>
   <si>
@@ -393,6 +390,18 @@
   </si>
   <si>
     <t>Vocals, Trombone</t>
+  </si>
+  <si>
+    <t>Greg</t>
+  </si>
+  <si>
+    <t>Walker</t>
+  </si>
+  <si>
+    <t>Pablo</t>
+  </si>
+  <si>
+    <t>Tellez</t>
   </si>
 </sst>
 </file>
@@ -424,7 +433,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -447,14 +456,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -735,11 +756,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -783,23 +813,21 @@
       <c r="F2" s="2">
         <v>1966</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="F3" s="2">
         <v>1966</v>
@@ -810,17 +838,17 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4" s="2">
         <v>1966</v>
@@ -831,17 +859,17 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F5" s="2">
         <v>1966</v>
@@ -852,19 +880,19 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="F6" s="2">
         <v>1967</v>
@@ -875,17 +903,17 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" s="2">
         <v>1969</v>
@@ -896,19 +924,19 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="F8" s="2">
         <v>1969</v>
@@ -919,17 +947,17 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F9" s="2">
         <v>1971</v>
@@ -940,17 +968,17 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F10" s="2">
         <v>1969</v>
@@ -961,17 +989,17 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>41</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F11" s="2">
         <v>1971</v>
@@ -982,17 +1010,17 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F12" s="2">
         <v>1971</v>
@@ -1003,17 +1031,17 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F13" s="2">
         <v>1972</v>
@@ -1024,17 +1052,17 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F14" s="2">
         <v>1972</v>
@@ -1045,17 +1073,17 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F15" s="2">
         <v>1972</v>
@@ -1066,17 +1094,17 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F16" s="2">
         <v>1972</v>
@@ -1087,19 +1115,19 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="D17" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F17" s="2">
         <v>1972</v>
@@ -1110,17 +1138,17 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F18" s="2">
         <v>1973</v>
@@ -1131,17 +1159,17 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F19" s="2">
         <v>1973</v>
@@ -1152,19 +1180,19 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="D20" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F20" s="2">
         <v>1974</v>
@@ -1175,500 +1203,490 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>17</v>
+        <v>121</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>64</v>
+        <v>122</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
       <c r="F21" s="2">
-        <v>1977</v>
+        <v>1976</v>
       </c>
       <c r="G21" s="2">
-        <v>1982</v>
+        <v>1978</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>65</v>
+        <v>16</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>67</v>
+        <v>14</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F22" s="2">
-        <v>1976</v>
+        <v>1977</v>
       </c>
       <c r="G22" s="2">
-        <v>1987</v>
+        <v>1982</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
-        <v>15</v>
+        <v>66</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F23" s="2">
         <v>1976</v>
       </c>
       <c r="G23" s="2">
-        <v>2013</v>
+        <v>1987</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>72</v>
+        <v>21</v>
       </c>
       <c r="F24" s="2">
-        <v>1978</v>
+        <v>1976</v>
       </c>
       <c r="G24" s="2">
-        <v>1980</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
-        <v>67</v>
+        <v>14</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F25" s="2">
-        <v>1979</v>
+        <v>1978</v>
       </c>
       <c r="G25" s="2">
-        <v>1994</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
-        <v>15</v>
+        <v>66</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="F26" s="2">
         <v>1979</v>
       </c>
       <c r="G26" s="2">
-        <v>1980</v>
+        <v>1994</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="F27" s="2">
+        <v>1979</v>
+      </c>
+      <c r="G27" s="2">
         <v>1980</v>
-      </c>
-      <c r="G27" s="2">
-        <v>1987</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="F28" s="2">
         <v>1980</v>
       </c>
       <c r="G28" s="2">
-        <v>1982</v>
+        <v>1987</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F29" s="2">
-        <v>1983</v>
+        <v>1980</v>
       </c>
       <c r="G29" s="2">
-        <v>2009</v>
+        <v>1982</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="F30" s="2">
-        <v>1985</v>
+        <v>1983</v>
       </c>
       <c r="G30" s="2">
-        <v>1991</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="F31" s="2">
         <v>1985</v>
       </c>
       <c r="G31" s="2">
-        <v>1986</v>
+        <v>1991</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="F32" s="2">
+        <v>1985</v>
+      </c>
+      <c r="G32" s="2">
         <v>1986</v>
-      </c>
-      <c r="G32" s="2">
-        <v>1987</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>28</v>
+        <v>88</v>
       </c>
       <c r="F33" s="2">
-        <v>1989</v>
+        <v>1986</v>
       </c>
       <c r="G33" s="2">
-        <v>1993</v>
+        <v>1987</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F34" s="2">
-        <v>1990</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>12</v>
+        <v>1989</v>
+      </c>
+      <c r="G34" s="2">
+        <v>1993</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
-        <v>15</v>
+        <v>93</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="F35" s="2">
-        <v>1991</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>12</v>
-      </c>
+        <v>1990</v>
+      </c>
+      <c r="G35" s="2"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="F36" s="2">
-        <v>1992</v>
-      </c>
-      <c r="G36" s="2">
-        <v>2005</v>
-      </c>
+        <v>1991</v>
+      </c>
+      <c r="G36" s="2"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F37" s="2">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="G37" s="2">
-        <v>2000</v>
+        <v>2005</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="F38" s="2">
-        <v>1995</v>
+        <v>1993</v>
       </c>
       <c r="G38" s="2">
-        <v>2015</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="F39" s="2">
-        <v>2002</v>
+        <v>1995</v>
       </c>
       <c r="G39" s="2">
-        <v>2013</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="F40" s="2">
-        <v>2000</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>12</v>
+        <v>2002</v>
+      </c>
+      <c r="G40" s="2">
+        <v>2013</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>109</v>
+        <v>60</v>
       </c>
       <c r="F41" s="2">
-        <v>2005</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>12</v>
-      </c>
+        <v>2000</v>
+      </c>
+      <c r="G41" s="2"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>17</v>
+        <v>106</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>51</v>
+        <v>108</v>
       </c>
       <c r="F42" s="2">
-        <v>2011</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>12</v>
-      </c>
+        <v>2005</v>
+      </c>
+      <c r="G42" s="2"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>111</v>
+        <v>16</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>113</v>
+        <v>50</v>
       </c>
       <c r="F43" s="2">
-        <v>2000</v>
-      </c>
-      <c r="G43" s="2">
-        <v>2016</v>
-      </c>
+        <v>2011</v>
+      </c>
+      <c r="G43" s="2"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F44" s="2">
         <v>2000</v>
@@ -1679,44 +1697,81 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>28</v>
+        <v>115</v>
       </c>
       <c r="F45" s="2">
-        <v>2010</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>12</v>
+        <v>2000</v>
+      </c>
+      <c r="G45" s="2">
+        <v>2016</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>121</v>
+        <v>27</v>
       </c>
       <c r="F46" s="2">
+        <v>2010</v>
+      </c>
+      <c r="G46" s="2"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F47" s="2">
         <v>2016</v>
       </c>
-      <c r="G46" s="2" t="s">
-        <v>12</v>
+      <c r="G47" s="2"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F48" s="3">
+        <v>1976</v>
+      </c>
+      <c r="G48" s="3">
+        <v>1977</v>
       </c>
     </row>
   </sheetData>

</xml_diff>